<commit_message>
Version 2.01: Overnight Trade Alerts
</commit_message>
<xml_diff>
--- a/2018-11-26 Cortex PnL.xlsx
+++ b/2018-11-26 Cortex PnL.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="17">
   <si>
     <t>Fees</t>
   </si>
@@ -40,13 +40,13 @@
     <t>Trades</t>
   </si>
   <si>
+    <t>BTCUSDT</t>
+  </si>
+  <si>
     <t>ETHUSDT</t>
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>BTCUSDT</t>
   </si>
   <si>
     <t>XRPUSDT</t>
@@ -476,7 +476,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -531,28 +531,28 @@
         <v>8</v>
       </c>
       <c r="B3" s="1">
-        <v>-0.0015</v>
+        <v>-0.0105</v>
       </c>
       <c r="C3" s="1">
-        <v>-0.00376334675301937</v>
+        <v>-0.002113275820349814</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="2">
-        <v>-0.07895020129529053</v>
+        <v>-0.5335401517879806</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H3" s="1">
-        <v>-0.005263346753019369</v>
+        <v>-0.01261327582034981</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -584,127 +584,127 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="3" t="s">
+    <row r="5" spans="1:9">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>-0.012</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-0.005876622573369183</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2">
+        <v>-0.6124903530832712</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1">
+        <v>-0.01787662257336918</v>
+      </c>
+      <c r="I5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="B9" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="B10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1">
-        <v>-0.0105</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.02320568303646275</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2">
-        <v>1.083534324903114</v>
-      </c>
-      <c r="G10">
-        <v>4</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0.01270568303646276</v>
-      </c>
-      <c r="I10">
+      <c r="I10" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1">
-        <v>-0.0015</v>
+        <v>-0.021</v>
       </c>
       <c r="C11" s="1">
-        <v>0.015610390666287</v>
+        <v>0.02109240721611294</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="2">
-        <v>0.211655859994305</v>
+        <v>1.357888248802745</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H11" s="1">
-        <v>0.014110390666287</v>
+        <v>9.240721611294533e-05</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>-0.0015</v>
       </c>
       <c r="C12" s="1">
-        <v>-0.00455107612827943</v>
+        <v>0.015610390666287</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12" s="2">
-        <v>-0.09076614192419144</v>
+        <v>0.211655859994305</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="1">
-        <v>-0.006051076128279429</v>
+        <v>0.014110390666287</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -712,13 +712,13 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>-0.0015</v>
       </c>
       <c r="C13" s="1">
-        <v>-0.00376334675301937</v>
+        <v>-0.00455107612827943</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -727,13 +727,13 @@
         <v>0</v>
       </c>
       <c r="F13" s="2">
-        <v>-0.07895020129529053</v>
+        <v>-0.09076614192419144</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13" s="1">
-        <v>-0.005263346753019369</v>
+        <v>-0.006051076128279429</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -741,212 +741,212 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B14" s="1">
-        <v>-0.003</v>
+        <v>-0.0015</v>
       </c>
       <c r="C14" s="1">
-        <v>-0.01426603576597285</v>
+        <v>-0.00376334675301937</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14" s="2">
-        <v>-0.4642147889812889</v>
+        <v>-0.07895020129529053</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14" s="1">
-        <v>-0.01726603576597285</v>
+        <v>-0.005263346753019369</v>
       </c>
       <c r="I14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1">
-        <v>-0.018</v>
+        <v>-0.003</v>
       </c>
       <c r="C15" s="1">
-        <v>0.0162356150554781</v>
+        <v>-0.01426603576597285</v>
       </c>
       <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>-0.4642147889812889</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>-0.01726603576597285</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="1">
+        <v>-0.0285</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.01412233923512829</v>
+      </c>
+      <c r="D16">
+        <v>12</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.9356129765962793</v>
+      </c>
+      <c r="G16">
         <v>7</v>
       </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2">
-        <v>0.6612590526966486</v>
-      </c>
-      <c r="G15">
+      <c r="H16" s="1">
+        <v>-0.01437766076487171</v>
+      </c>
+      <c r="I16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="B21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H15" s="1">
-        <v>-0.001764384944521897</v>
-      </c>
-      <c r="I15">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="B20" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H20" s="4" t="s">
+      <c r="H21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="I21" s="4" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="1">
-        <v>-0.03600000000000001</v>
-      </c>
-      <c r="C21" s="1">
-        <v>0.01486902881877017</v>
-      </c>
-      <c r="D21">
-        <v>16</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21" s="2">
-        <v>-3.58225354593918</v>
-      </c>
-      <c r="G21">
-        <v>8</v>
-      </c>
-      <c r="H21" s="1">
-        <v>-0.02113097118122984</v>
-      </c>
-      <c r="I21">
-        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B22" s="1">
-        <v>-0.08100000000000004</v>
+        <v>-0.04650000000000002</v>
       </c>
       <c r="C22" s="1">
-        <v>-0.04209248219239115</v>
+        <v>0.01275575299842036</v>
       </c>
       <c r="D22">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="2">
-        <v>-32.90939318678556</v>
+        <v>-6.463717515209433</v>
       </c>
       <c r="G22">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H22" s="1">
-        <v>-0.1230924821923912</v>
+        <v>-0.03374424700157966</v>
       </c>
       <c r="I22">
-        <v>54</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B23" s="1">
-        <v>-0.0015</v>
+        <v>-0.08100000000000004</v>
       </c>
       <c r="C23" s="1">
-        <v>0.015610390666287</v>
+        <v>-0.04209248219239115</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23" s="2">
-        <v>0.211655859994305</v>
+        <v>-32.90939318678556</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H23" s="1">
-        <v>0.014110390666287</v>
+        <v>-0.1230924821923912</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B24" s="1">
         <v>-0.0015</v>
       </c>
       <c r="C24" s="1">
-        <v>-0.00455107612827943</v>
+        <v>0.015610390666287</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="F24" s="2">
-        <v>-0.09076614192419144</v>
+        <v>0.211655859994305</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="1">
-        <v>-0.006051076128279429</v>
+        <v>0.014110390666287</v>
       </c>
       <c r="I24">
         <v>1</v>
@@ -954,31 +954,31 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B25" s="1">
-        <v>-0.003</v>
+        <v>-0.0015</v>
       </c>
       <c r="C25" s="1">
-        <v>-0.009020822225957459</v>
+        <v>-0.00455107612827943</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25" s="2">
-        <v>-0.1390543124250778</v>
+        <v>-0.09076614192419144</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25" s="1">
-        <v>-0.01202082222595746</v>
+        <v>-0.006051076128279429</v>
       </c>
       <c r="I25">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -986,52 +986,81 @@
         <v>9</v>
       </c>
       <c r="B26" s="1">
-        <v>-0.1230000000000001</v>
+        <v>-0.003</v>
       </c>
       <c r="C26" s="1">
-        <v>-0.02518496106157087</v>
+        <v>-0.009020822225957459</v>
       </c>
       <c r="D26">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
       <c r="F26" s="2">
-        <v>-36.50981132707972</v>
+        <v>-0.1390543124250778</v>
       </c>
       <c r="G26">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H26" s="1">
-        <v>-0.1481849610615709</v>
+        <v>-0.01202082222595746</v>
       </c>
       <c r="I26">
-        <v>82</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="1">
+        <v>-0.1335000000000001</v>
+      </c>
+      <c r="C27" s="1">
+        <v>-0.02729823688192068</v>
+      </c>
+      <c r="D27">
+        <v>71</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2">
+        <v>-39.39127529634997</v>
+      </c>
+      <c r="G27">
+        <v>18</v>
+      </c>
+      <c r="H27" s="1">
+        <v>-0.1607982368819207</v>
+      </c>
+      <c r="I27">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="A19:I19"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="A20:I20"/>
   </mergeCells>
-  <conditionalFormatting sqref="A15:I15">
+  <conditionalFormatting sqref="A16:I16">
     <cfRule type="notContainsErrors" dxfId="2" priority="6">
-      <formula>NOT(ISERROR(A15))</formula>
+      <formula>NOT(ISERROR(A16))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A26:I26">
+  <conditionalFormatting sqref="A27:I27">
     <cfRule type="notContainsErrors" dxfId="2" priority="9">
-      <formula>NOT(ISERROR(A26))</formula>
+      <formula>NOT(ISERROR(A27))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4:I4">
+  <conditionalFormatting sqref="A5:I5">
     <cfRule type="notContainsErrors" dxfId="2" priority="3">
-      <formula>NOT(ISERROR(A4))</formula>
+      <formula>NOT(ISERROR(A5))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H10:H14">
+  <conditionalFormatting sqref="H11:H15">
     <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -1039,7 +1068,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H21:H25">
+  <conditionalFormatting sqref="H22:H26">
     <cfRule type="cellIs" dxfId="0" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -1047,7 +1076,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3">
+  <conditionalFormatting sqref="H3:H4">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>